<commit_message>
Phase 2 Pi Push
</commit_message>
<xml_diff>
--- a/studentMaster.xlsx
+++ b/studentMaster.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Student Details" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Programme Name</t>
   </si>
@@ -49,12 +49,24 @@
   </si>
   <si>
     <t>Sanjeev Kanth S</t>
+  </si>
+  <si>
+    <t>Ramya P</t>
+  </si>
+  <si>
+    <t>Rajakumaran Bhavanishraj</t>
+  </si>
+  <si>
+    <t>Keerthivasan S</t>
+  </si>
+  <si>
+    <t>Hareesh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,21 +413,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -437,65 +449,121 @@
         <v>2022</v>
       </c>
       <c r="C2" s="3">
+        <v>220701128</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C3" s="3">
+        <v>220701079</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C4" s="3">
+        <v>220701217</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C5" s="3">
+        <v>220701215</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C6" s="3">
         <v>220701222</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2022</v>
-      </c>
-      <c r="C3" s="3">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C7" s="3">
         <v>220701236</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2022</v>
-      </c>
-      <c r="C4" s="3">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C8" s="3">
         <v>220701237</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2">
-        <v>2022</v>
-      </c>
-      <c r="C5" s="3">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C9" s="3">
         <v>220701250</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2022</v>
-      </c>
-      <c r="C6" s="3">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C10" s="3">
         <v>220701251</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>